<commit_message>
Rewritten MacrofractureXYZ.PopulateData() to bevel segment corners only if the I coordinate of the crossover point between the edges of adjacent segments lies between the I coordinate of the two segment cornerpoints, rather than using a minimum angle cutoff (B84), but not yet tested. Modified FractureSet.checkStressShadowInteraction() to not create relay zones if a third fracture lies between the two fracture tips (B85), but not yet working.
</commit_message>
<xml_diff>
--- a/Documentation/WorkToDo.xlsx
+++ b/Documentation/WorkToDo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MWelch\source\repos\DFMGenerator_Code2\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MWelch\source\repos\DFMGenerator_Code\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649384D4-B3D9-499C-9706-48DADE7D3D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A437ED1B-A6A2-4E79-AF1D-DB242F6C76C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bug fixes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="584">
   <si>
     <t>Type</t>
   </si>
@@ -1249,9 +1249,6 @@
     <t>D19</t>
   </si>
   <si>
-    <t>Write a short installation and use guide to Petrel plugin for DUC users</t>
-  </si>
-  <si>
     <t>Write a short installation and use guide to standalone version for Github</t>
   </si>
   <si>
@@ -1950,6 +1947,33 @@
   </si>
   <si>
     <t>Needs testing</t>
+  </si>
+  <si>
+    <t>B84</t>
+  </si>
+  <si>
+    <t>Write a short installation and use guide to Petrel plugin version</t>
+  </si>
+  <si>
+    <t>Still producing "spiking" fractures in explicit DFN</t>
+  </si>
+  <si>
+    <t>Done; needs testing using Gullfaks Workflow 2</t>
+  </si>
+  <si>
+    <t>B85</t>
+  </si>
+  <si>
+    <t>Generating small patches of highly intense fracturing near edges of gridblocks</t>
+  </si>
+  <si>
+    <t>Done but not yet working</t>
+  </si>
+  <si>
+    <t>When run with oblique fracture sets, it occasionally still produces "spiking" factures (where one or more cornerpoints lies way outside the model bounds). This is probably due to trying to bevel two nearly parallel fracture segment edges. Rewritten MacrofractureXYZ.PopulateData() to bevel only if the I coordinate of the crossover point between the edges of adjacent segments lies between the I coordinate of the two segment cornerpoints, rather than using a minimum angle cutoff.</t>
+  </si>
+  <si>
+    <t>When run with oblique fracture sets, it often generates small patches at the edges of gridblocks with very intense, closely spaced fracture segments. It appears that these are mostly relay segments rather than propagating segments; the intense zones contain only one or two fractures, but these are made up of very short segments connected by relay zones. The patches are probably gaps between the stress shadows of primary fractures, where only later non-optimally aligned fractures can grow. However the relay zones often cross each other. This can be fixed by modifying FractureSet.checkStressShadowInteraction() to not create relay zones if a third fracture lies between the two fracture tips.</t>
   </si>
 </sst>
 </file>
@@ -2378,11 +2402,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I90"/>
+  <dimension ref="A1:I92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G82" sqref="G82"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2594,7 +2618,7 @@
         <v>36</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2918,7 +2942,7 @@
         <v>38</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -3326,7 +3350,7 @@
         <v>258</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F41" s="3">
         <v>0.5</v>
@@ -3372,7 +3396,7 @@
         <v>261</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F43" s="3">
         <v>0.25</v>
@@ -3628,16 +3652,16 @@
     </row>
     <row r="54" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C54" s="4" t="s">
+      <c r="D54" s="4" t="s">
         <v>349</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>350</v>
       </c>
       <c r="F54" s="3">
         <v>1</v>
@@ -3651,16 +3675,16 @@
     </row>
     <row r="55" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C55" s="4" t="s">
+      <c r="D55" s="4" t="s">
         <v>352</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>353</v>
       </c>
       <c r="F55" s="3">
         <v>0.5</v>
@@ -3674,22 +3698,22 @@
     </row>
     <row r="56" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C56" s="4" t="s">
+      <c r="D56" s="4" t="s">
         <v>383</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>384</v>
       </c>
       <c r="F56" s="3">
         <v>0.5</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>36</v>
@@ -3700,22 +3724,22 @@
     </row>
     <row r="57" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C57" s="4" t="s">
+      <c r="D57" s="4" t="s">
         <v>387</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>388</v>
       </c>
       <c r="F57" s="3">
         <v>0.5</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H57" s="3" t="s">
         <v>36</v>
@@ -3726,22 +3750,22 @@
     </row>
     <row r="58" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>390</v>
-      </c>
       <c r="D58" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F58" s="3">
         <v>0.5</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>38</v>
@@ -3752,22 +3776,22 @@
     </row>
     <row r="59" spans="1:9" s="3" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>398</v>
-      </c>
       <c r="D59" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F59" s="3">
         <v>0.5</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H59" s="3" t="s">
         <v>36</v>
@@ -3778,22 +3802,22 @@
     </row>
     <row r="60" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C60" s="4" t="s">
+      <c r="D60" s="4" t="s">
         <v>404</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>405</v>
       </c>
       <c r="F60" s="3">
         <v>0.5</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>36</v>
@@ -3804,22 +3828,22 @@
     </row>
     <row r="61" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C61" s="4" t="s">
+      <c r="D61" s="4" t="s">
         <v>408</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>409</v>
       </c>
       <c r="F61" s="3">
         <v>0.5</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H61" s="3" t="s">
         <v>36</v>
@@ -3830,22 +3854,22 @@
     </row>
     <row r="62" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C62" s="4" t="s">
+      <c r="D62" s="4" t="s">
         <v>411</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>412</v>
       </c>
       <c r="F62" s="3">
         <v>1</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>36</v>
@@ -3856,22 +3880,22 @@
     </row>
     <row r="63" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C63" s="4" t="s">
+      <c r="D63" s="4" t="s">
         <v>425</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>426</v>
       </c>
       <c r="F63" s="3">
         <v>0.5</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H63" s="3" t="s">
         <v>38</v>
@@ -3882,16 +3906,16 @@
     </row>
     <row r="64" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>429</v>
-      </c>
       <c r="D64" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F64" s="3">
         <v>0.5</v>
@@ -3900,21 +3924,21 @@
         <v>36</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C65" s="4" t="s">
+      <c r="D65" s="4" t="s">
         <v>434</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>435</v>
       </c>
       <c r="F65" s="3">
         <v>0.5</v>
@@ -3923,21 +3947,21 @@
         <v>38</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F66" s="3">
         <v>0.25</v>
@@ -3946,21 +3970,21 @@
         <v>38</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C67" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="D67" s="4" t="s">
         <v>442</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>443</v>
       </c>
       <c r="F67" s="3">
         <v>0.25</v>
@@ -3969,605 +3993,651 @@
         <v>36</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F68" s="3">
         <v>1</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C69" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="D69" s="4" t="s">
         <v>445</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>446</v>
       </c>
       <c r="F69" s="3">
         <v>0.25</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H69" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F70" s="3">
         <v>0.25</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H70" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="71" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F71" s="3">
         <v>0.5</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H71" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C72" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="D72" s="4" t="s">
         <v>451</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>452</v>
       </c>
       <c r="F72" s="3">
         <v>0.25</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F73" s="3">
         <v>0.25</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H73" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="4" t="s">
         <v>460</v>
       </c>
-      <c r="B74" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C74" s="4" t="s">
+      <c r="D74" s="4" t="s">
         <v>461</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>462</v>
       </c>
       <c r="F74" s="3">
         <v>0.25</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" s="4" t="s">
         <v>463</v>
       </c>
-      <c r="B75" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C75" s="4" t="s">
+      <c r="D75" s="4" t="s">
         <v>464</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>465</v>
       </c>
       <c r="F75" s="3">
         <v>0.5</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H75" s="3" t="s">
         <v>38</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" s="4" t="s">
         <v>467</v>
       </c>
-      <c r="B76" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C76" s="4" t="s">
+      <c r="D76" s="4" t="s">
         <v>468</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>469</v>
       </c>
       <c r="F76" s="3">
         <v>0.25</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>38</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="77" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C77" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="B77" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>481</v>
-      </c>
       <c r="D77" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F77" s="3">
         <v>0.5</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H77" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="78" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C78" s="4" t="s">
         <v>488</v>
       </c>
-      <c r="B78" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C78" s="4" t="s">
+      <c r="D78" s="4" t="s">
         <v>489</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>490</v>
       </c>
       <c r="F78" s="3">
         <v>0.25</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>38</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="79" spans="1:9" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C79" s="4" t="s">
         <v>491</v>
       </c>
-      <c r="B79" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C79" s="4" t="s">
+      <c r="D79" s="4" t="s">
         <v>492</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>493</v>
       </c>
       <c r="F79" s="3">
         <v>1</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H79" s="3" t="s">
         <v>38</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="80" spans="1:9" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C80" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="B80" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C80" s="4" t="s">
+      <c r="D80" s="4" t="s">
         <v>505</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>506</v>
       </c>
       <c r="F80" s="3">
         <v>0.5</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="81" spans="1:9" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C81" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="B81" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>508</v>
-      </c>
       <c r="D81" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F81" s="3">
         <v>1</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H81" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="82" spans="1:9" s="6" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C82" s="7" t="s">
         <v>509</v>
       </c>
-      <c r="B82" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>510</v>
-      </c>
       <c r="D82" s="7" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F82" s="6">
         <v>1</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H82" s="6" t="s">
         <v>36</v>
       </c>
       <c r="I82" s="6" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="83" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83" s="4" t="s">
         <v>511</v>
       </c>
-      <c r="B83" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C83" s="4" t="s">
+      <c r="D83" s="4" t="s">
         <v>512</v>
-      </c>
-      <c r="D83" s="4" t="s">
-        <v>513</v>
       </c>
       <c r="F83" s="3">
         <v>0.5</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H83" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="84" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="B84" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>515</v>
-      </c>
       <c r="D84" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F84" s="3">
         <v>0.5</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="B85" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>527</v>
-      </c>
       <c r="D85" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F85" s="1">
         <v>0.5</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>36</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="86" spans="1:9" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="B86" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C86" s="4" t="s">
+      <c r="D86" s="4" t="s">
         <v>532</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>533</v>
       </c>
       <c r="F86" s="3">
         <v>0.5</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="87" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="B87" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C87" s="4" t="s">
+      <c r="D87" s="4" t="s">
         <v>540</v>
-      </c>
-      <c r="D87" s="4" t="s">
-        <v>541</v>
       </c>
       <c r="F87" s="3">
         <v>0.5</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H87" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="88" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C88" s="4" t="s">
         <v>542</v>
       </c>
-      <c r="B88" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C88" s="4" t="s">
+      <c r="D88" s="4" t="s">
         <v>543</v>
-      </c>
-      <c r="D88" s="4" t="s">
-        <v>544</v>
       </c>
       <c r="F88" s="3">
         <v>0.5</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H88" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="89" spans="1:9" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C89" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="B89" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C89" s="4" t="s">
+      <c r="D89" s="4" t="s">
         <v>546</v>
-      </c>
-      <c r="D89" s="4" t="s">
-        <v>547</v>
       </c>
       <c r="F89" s="3">
         <v>1</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H89" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="90" spans="1:9" s="3" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="D90" s="4" t="s">
         <v>548</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>546</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>549</v>
       </c>
       <c r="F90" s="3">
         <v>1</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A91" s="6" t="s">
+        <v>575</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>577</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="F91" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="H91" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I91" s="6" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A92" s="8" t="s">
+        <v>579</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>580</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="F92" s="8">
+        <v>1</v>
+      </c>
+      <c r="H92" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I92" s="8" t="s">
+        <v>581</v>
       </c>
     </row>
   </sheetData>
@@ -4584,7 +4654,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -4742,10 +4812,10 @@
         <v>20</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -4837,10 +4907,10 @@
         <v>0.25</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -5047,7 +5117,7 @@
         <v>38</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -5314,16 +5384,16 @@
     </row>
     <row r="31" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>355</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>356</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
@@ -5334,16 +5404,16 @@
     </row>
     <row r="32" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C32" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>367</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>368</v>
       </c>
       <c r="F32" s="3">
         <v>0.5</v>
@@ -5360,16 +5430,16 @@
     </row>
     <row r="33" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C33" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>361</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>362</v>
       </c>
       <c r="F33" s="3">
         <v>1</v>
@@ -5386,16 +5456,16 @@
     </row>
     <row r="34" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>364</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>365</v>
       </c>
       <c r="F34" s="3">
         <v>0.5</v>
@@ -5412,16 +5482,16 @@
     </row>
     <row r="35" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F35" s="3">
         <v>1</v>
@@ -5438,16 +5508,16 @@
     </row>
     <row r="36" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>370</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>371</v>
       </c>
       <c r="F36" s="3">
         <v>0.5</v>
@@ -5464,16 +5534,16 @@
     </row>
     <row r="37" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C37" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>376</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>377</v>
       </c>
       <c r="F37" s="3">
         <v>0.5</v>
@@ -5490,16 +5560,16 @@
     </row>
     <row r="38" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C38" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>373</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>374</v>
       </c>
       <c r="F38" s="3">
         <v>1</v>
@@ -5516,16 +5586,16 @@
     </row>
     <row r="39" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F39" s="1">
         <v>1</v>
@@ -5534,21 +5604,21 @@
         <v>37</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C40" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>393</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>394</v>
       </c>
       <c r="F40" s="3">
         <v>1</v>
@@ -5565,38 +5635,38 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>502</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C43" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>391</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>392</v>
       </c>
       <c r="F43" s="3">
         <v>0.5</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H43" s="3" t="s">
         <v>38</v>
@@ -5607,22 +5677,22 @@
     </row>
     <row r="44" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C44" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>401</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>402</v>
       </c>
       <c r="F44" s="3">
         <v>0.2</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>38</v>
@@ -5633,16 +5703,16 @@
     </row>
     <row r="45" spans="1:9" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B45" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C45" s="13" t="s">
+        <v>436</v>
+      </c>
+      <c r="D45" s="13" t="s">
         <v>437</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>438</v>
       </c>
       <c r="F45" s="12">
         <v>0.2</v>
@@ -5656,16 +5726,16 @@
     </row>
     <row r="46" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C46" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>471</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>472</v>
       </c>
       <c r="F46" s="3">
         <v>0.2</v>
@@ -5674,21 +5744,21 @@
         <v>38</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C47" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="D47" s="4" t="s">
         <v>495</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>496</v>
       </c>
       <c r="F47" s="3">
         <v>0.5</v>
@@ -5697,21 +5767,21 @@
         <v>38</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C48" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="D48" s="4" t="s">
         <v>498</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>499</v>
       </c>
       <c r="F48" s="3">
         <v>0.1</v>
@@ -5720,21 +5790,21 @@
         <v>38</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C49" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>520</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>521</v>
       </c>
       <c r="F49" s="3">
         <v>2</v>
@@ -5743,27 +5813,27 @@
         <v>36</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B50" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C50" s="15" t="s">
+        <v>522</v>
+      </c>
+      <c r="D50" s="15" t="s">
         <v>523</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="F50" s="14">
+        <v>3</v>
+      </c>
+      <c r="G50" s="14" t="s">
         <v>524</v>
-      </c>
-      <c r="F50" s="14">
-        <v>3</v>
-      </c>
-      <c r="G50" s="14" t="s">
-        <v>525</v>
       </c>
       <c r="H50" s="14" t="s">
         <v>36</v>
@@ -5771,16 +5841,16 @@
     </row>
     <row r="51" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C51" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>535</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>536</v>
       </c>
       <c r="F51" s="3">
         <v>1</v>
@@ -5794,16 +5864,16 @@
     </row>
     <row r="52" spans="1:9" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C52" s="7" t="s">
+        <v>536</v>
+      </c>
+      <c r="D52" s="7" t="s">
         <v>537</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>538</v>
       </c>
       <c r="F52" s="6">
         <v>0.5</v>
@@ -5814,16 +5884,16 @@
     </row>
     <row r="53" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C53" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>552</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>553</v>
       </c>
       <c r="F53" s="3">
         <v>0.5</v>
@@ -5848,8 +5918,8 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6096,7 +6166,7 @@
         <v>38</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -6119,7 +6189,7 @@
         <v>36</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -6309,7 +6379,7 @@
         <v>325</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>342</v>
+        <v>576</v>
       </c>
       <c r="F18" s="3">
         <v>1</v>
@@ -6332,7 +6402,7 @@
         <v>325</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F19" s="3">
         <v>1</v>
@@ -6352,7 +6422,7 @@
         <v>45</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>340</v>
@@ -6369,16 +6439,16 @@
     </row>
     <row r="21" spans="1:9" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C21" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>345</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>346</v>
       </c>
       <c r="F21" s="8">
         <v>2</v>
@@ -6389,16 +6459,16 @@
     </row>
     <row r="22" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F22" s="3">
         <v>1</v>
@@ -6488,7 +6558,7 @@
         <v>37</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6528,19 +6598,19 @@
         <v>77</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F4" s="14">
         <v>50</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>36</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -6554,7 +6624,7 @@
         <v>240</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F5" s="3">
         <v>2</v>
@@ -6577,7 +6647,7 @@
         <v>260</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F6" s="3">
         <v>2</v>
@@ -6591,42 +6661,42 @@
     </row>
     <row r="7" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>414</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>415</v>
       </c>
       <c r="F7" s="3">
         <v>5</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>420</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>421</v>
       </c>
       <c r="F8" s="1">
         <v>10</v>
@@ -6635,47 +6705,47 @@
         <v>37</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>431</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>432</v>
       </c>
       <c r="F9" s="3">
         <v>5</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>478</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>479</v>
       </c>
       <c r="F10" s="1">
         <v>10</v>
@@ -6684,21 +6754,21 @@
         <v>37</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>83</v>
       </c>
       <c r="C11" s="15" t="s">
+        <v>517</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>518</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>519</v>
       </c>
       <c r="F11" s="14">
         <f>20*12</f>
@@ -6708,7 +6778,7 @@
         <v>37</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified Gridblock.ExtendFracture() to add relay fracture segments to the list of local macrofracture segments in eash fracture set object (although not the list of MacrofractureSegmentHolders in each gridblock object) to allow cross-checking (B85).
</commit_message>
<xml_diff>
--- a/Documentation/WorkToDo.xlsx
+++ b/Documentation/WorkToDo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MWelch\source\repos\DFMGenerator_Code\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joint\source\repos\DFMGenerator_Code\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A437ED1B-A6A2-4E79-AF1D-DB242F6C76C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02ECE459-2292-4325-8D1A-5D3A7F972601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bug fixes" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="583">
   <si>
     <t>Type</t>
   </si>
@@ -1967,13 +1965,10 @@
     <t>Generating small patches of highly intense fracturing near edges of gridblocks</t>
   </si>
   <si>
-    <t>Done but not yet working</t>
-  </si>
-  <si>
     <t>When run with oblique fracture sets, it occasionally still produces "spiking" factures (where one or more cornerpoints lies way outside the model bounds). This is probably due to trying to bevel two nearly parallel fracture segment edges. Rewritten MacrofractureXYZ.PopulateData() to bevel only if the I coordinate of the crossover point between the edges of adjacent segments lies between the I coordinate of the two segment cornerpoints, rather than using a minimum angle cutoff.</t>
   </si>
   <si>
-    <t>When run with oblique fracture sets, it often generates small patches at the edges of gridblocks with very intense, closely spaced fracture segments. It appears that these are mostly relay segments rather than propagating segments; the intense zones contain only one or two fractures, but these are made up of very short segments connected by relay zones. The patches are probably gaps between the stress shadows of primary fractures, where only later non-optimally aligned fractures can grow. However the relay zones often cross each other. This can be fixed by modifying FractureSet.checkStressShadowInteraction() to not create relay zones if a third fracture lies between the two fracture tips.</t>
+    <t>When run with oblique fracture sets, it often generates small patches at the edges of gridblocks with very intense, closely spaced fracture segments. It appears that these are mostly relay segments rather than propagating segments; the intense zones contain only one or two fractures, but these are made up of very short segments connected by relay zones. The patches represent gaps between the stress shadows of primary fractures and the edges of the grid, or between the stress shadows of misaligned primary fractures in adjacent gridblocks, where only later non-optimally aligned fractures can grow. This cannot be prevented; however the relay zones often cross each other. This problem can be fixed by modifying FractureSet.checkStressShadowInteraction() to not create relay zones if a third fracture lies between the two fracture tips. It was also necessary to add relay fracture segments to the list of local macrofracture segments in eash fracture set object (although not the list of MacrofractureSegmentHolders in each gridblock object) to allow cross-checking.</t>
   </si>
 </sst>
 </file>
@@ -2405,8 +2400,8 @@
   <dimension ref="A1:I92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D93" sqref="D93"/>
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A91" sqref="A91:XFD92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4605,7 +4600,7 @@
         <v>577</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F91" s="6">
         <v>0.5</v>
@@ -4617,27 +4612,27 @@
         <v>578</v>
       </c>
     </row>
-    <row r="92" spans="1:9" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A92" s="8" t="s">
+    <row r="92" spans="1:9" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
         <v>579</v>
       </c>
-      <c r="B92" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C92" s="9" t="s">
+      <c r="B92" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92" s="7" t="s">
         <v>580</v>
       </c>
-      <c r="D92" s="9" t="s">
-        <v>583</v>
-      </c>
-      <c r="F92" s="8">
+      <c r="D92" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="F92" s="6">
         <v>1</v>
       </c>
-      <c r="H92" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="I92" s="8" t="s">
-        <v>581</v>
+      <c r="H92" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I92" s="6" t="s">
+        <v>578</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created a list of XYZ centrepoints within the MacrofractureXYZ object and populate this in the PopulateData() function, as the fracture patch cornerpoints are; since this is called at the end of each stage, it will populate it with the centrepoint locations at that time, so there will be no mismatch between the centrepoint and segments of the early stages of the DFN if individual segments continue to grow, as occurs if the centrepoints simply reference still active MacrofractureSegmentIJK nodes (B86).
</commit_message>
<xml_diff>
--- a/Documentation/WorkToDo.xlsx
+++ b/Documentation/WorkToDo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joint\source\repos\DFMGenerator_Code\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MWelch\source\repos\DFMGenerator_Code\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02ECE459-2292-4325-8D1A-5D3A7F972601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF43E88F-0727-4CD2-9875-044A4E05515C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bug fixes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="585">
   <si>
     <t>Type</t>
   </si>
@@ -1727,9 +1727,6 @@
     <t>ME49</t>
   </si>
   <si>
-    <t>Not relevant for OS release</t>
-  </si>
-  <si>
     <t>B73</t>
   </si>
   <si>
@@ -1941,12 +1938,6 @@
     <t>Needs fixing for CCS applications</t>
   </si>
   <si>
-    <t>This is due to the new code that allows the fracture dipset evolution stage to revert from Residual to Growing in FractureDipSet.calculateTotalMacrofracturePopulation(). When this happened it was not resetting the density increments to zero. This was especially a problem for the s_MFP30_increment, which was getting multiplied by the timestep duration twice and leading to very large increments. This has been fixed, but still need to check if 1) does this also affect calculateMacrofractureArrays() fn?, 2) Does this problem occur anywhere else, 3) When and why does the state sometimes oscillate between Residual and Growing, even with no vertical extension?, 4) A few cells (e.g. 24,21 in Gullfaks Tarbert 2) still do not form secondary sets in the new code, whereas they did in the old.  This occurs because the test for switching from Growing to Residual (residual aMFP30 &gt; growing aMFP30) is not the same as the test for reverting from Residual to Growing (maximum propagation length in timestep &gt; mean propagation length before deactivating). Modified the code so it does not revert from ResidualActive to Growing within the calculateTotalMacrofracturePopulation() function, but instead within the fds.checkStressShadowWidthChange() function, only if the stress shadow width has changed. This fixes the problem but still needs testing on multi-stage models</t>
-  </si>
-  <si>
-    <t>Needs testing</t>
-  </si>
-  <si>
     <t>B84</t>
   </si>
   <si>
@@ -1956,19 +1947,34 @@
     <t>Still producing "spiking" fractures in explicit DFN</t>
   </si>
   <si>
-    <t>Done; needs testing using Gullfaks Workflow 2</t>
-  </si>
-  <si>
     <t>B85</t>
   </si>
   <si>
     <t>Generating small patches of highly intense fracturing near edges of gridblocks</t>
   </si>
   <si>
-    <t>When run with oblique fracture sets, it occasionally still produces "spiking" factures (where one or more cornerpoints lies way outside the model bounds). This is probably due to trying to bevel two nearly parallel fracture segment edges. Rewritten MacrofractureXYZ.PopulateData() to bevel only if the I coordinate of the crossover point between the edges of adjacent segments lies between the I coordinate of the two segment cornerpoints, rather than using a minimum angle cutoff.</t>
-  </si>
-  <si>
     <t>When run with oblique fracture sets, it often generates small patches at the edges of gridblocks with very intense, closely spaced fracture segments. It appears that these are mostly relay segments rather than propagating segments; the intense zones contain only one or two fractures, but these are made up of very short segments connected by relay zones. The patches represent gaps between the stress shadows of primary fractures and the edges of the grid, or between the stress shadows of misaligned primary fractures in adjacent gridblocks, where only later non-optimally aligned fractures can grow. This cannot be prevented; however the relay zones often cross each other. This problem can be fixed by modifying FractureSet.checkStressShadowInteraction() to not create relay zones if a third fracture lies between the two fracture tips. It was also necessary to add relay fracture segments to the list of local macrofracture segments in eash fracture set object (although not the list of MacrofractureSegmentHolders in each gridblock object) to allow cross-checking.</t>
+  </si>
+  <si>
+    <t>When run with oblique fracture sets, it occasionally still produces "spiking" factures (where one or more cornerpoints lies way outside the model bounds). This is due to trying to bevel against a nearly parallel intersecting fracture segment edges. Rewritten MacrofractureXYZ.PopulateData() and PointXYZ.getCrossoverPoint() to allow limits to the bevelling relative to the fracture segment against which it is bevelled (both for intersecting fractures and other segments of the same fracture), rather than using a minimum angle cutoff.</t>
+  </si>
+  <si>
+    <t>This is due to the new code that allows the fracture dipset evolution stage to revert from Residual to Growing in FractureDipSet.calculateTotalMacrofracturePopulation(). When this happened it was not resetting the density increments to zero. This was especially a problem for the s_MFP30_increment, which was getting multiplied by the timestep duration twice and leading to very large increments. This has been fixed, but still need to check if 1) does this also affect calculateMacrofractureArrays() fn?, 2) Does this problem occur anywhere else, 3) When and why does the state sometimes oscillate between Residual and Growing, even with no vertical extension?, 4) A few cells (e.g. 24,21 in Gullfaks Tarbert 2) still do not form secondary sets in the new code, whereas they did in the old.  This occurs because the test for switching from Growing to Residual (residual aMFP30 &gt; growing aMFP30) is not the same as the test for reverting from Residual to Growing (maximum propagation length in timestep &gt; mean propagation length before deactivating). Modified the code so it does not revert from ResidualActive to Growing within the calculateTotalMacrofracturePopulation() function, but instead within the fds.checkStressShadowWidthChange() function, only if the stress shadow width has changed.</t>
+  </si>
+  <si>
+    <t>Not relevant for OS release</t>
+  </si>
+  <si>
+    <t>B86</t>
+  </si>
+  <si>
+    <t>Centrelines do not match DFN fracture patches in multistage Petrel models</t>
+  </si>
+  <si>
+    <t>When multistage Petrel models are run with fractures growing within each gridblock in between output stages, the output centrelines are consistently longer than the fracture patches in the early output stages. This problem does not affect output files, in which the centrelines are consistent with the fracture patches. This is because the copies of the global DFN that are made at the end of each stage contain links to the still active local MacrofractureSegmentIJK objects rather than inactive copies of these; if the segments subsequently grow, these longer versions will be used to populate the centrelines in the Petrel model (which is done after the explicit DFN growth has run to completion). The problem can be solved by creating a list of XYZ centrepoints within the MacrofractureXYZ object and populating this in the PopulateData function, as the fracture patch cornerpoints are; since this is called at the end of each stage, it will populate it with the centrepoint locations at that time.</t>
+  </si>
+  <si>
+    <t>For Release 2.2.3</t>
   </si>
 </sst>
 </file>
@@ -2397,11 +2403,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I92"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A91" sqref="A91:XFD92"/>
+      <selection pane="bottomLeft" activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2613,7 +2619,7 @@
         <v>36</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2937,7 +2943,7 @@
         <v>38</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -3391,7 +3397,7 @@
         <v>261</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F43" s="3">
         <v>0.25</v>
@@ -4002,13 +4008,13 @@
         <v>443</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F68" s="3">
         <v>1</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>36</v>
@@ -4034,7 +4040,7 @@
         <v>0.25</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H69" s="3" t="s">
         <v>36</v>
@@ -4060,7 +4066,7 @@
         <v>0.25</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H70" s="3" t="s">
         <v>36</v>
@@ -4086,7 +4092,7 @@
         <v>0.5</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H71" s="3" t="s">
         <v>36</v>
@@ -4112,7 +4118,7 @@
         <v>0.25</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>36</v>
@@ -4138,7 +4144,7 @@
         <v>0.25</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H73" s="3" t="s">
         <v>36</v>
@@ -4164,7 +4170,7 @@
         <v>0.25</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>36</v>
@@ -4305,16 +4311,16 @@
     </row>
     <row r="80" spans="1:9" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C80" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="B80" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C80" s="4" t="s">
+      <c r="D80" s="4" t="s">
         <v>504</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>505</v>
       </c>
       <c r="F80" s="3">
         <v>0.5</v>
@@ -4326,21 +4332,21 @@
         <v>36</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="81" spans="1:9" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C81" s="4" t="s">
         <v>506</v>
       </c>
-      <c r="B81" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>507</v>
-      </c>
       <c r="D81" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F81" s="3">
         <v>1</v>
@@ -4352,47 +4358,47 @@
         <v>36</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" s="6" customFormat="1" ht="210" x14ac:dyDescent="0.25">
-      <c r="A82" s="6" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" s="3" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C82" s="4" t="s">
         <v>508</v>
       </c>
-      <c r="B82" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>509</v>
-      </c>
-      <c r="D82" s="7" t="s">
-        <v>573</v>
-      </c>
-      <c r="F82" s="6">
+      <c r="D82" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="F82" s="3">
         <v>1</v>
       </c>
-      <c r="G82" s="6" t="s">
+      <c r="G82" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="H82" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I82" s="6" t="s">
-        <v>574</v>
+      <c r="H82" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I82" s="3" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="83" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="B83" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C83" s="4" t="s">
+      <c r="D83" s="4" t="s">
         <v>511</v>
-      </c>
-      <c r="D83" s="4" t="s">
-        <v>512</v>
       </c>
       <c r="F83" s="3">
         <v>0.5</v>
@@ -4404,21 +4410,21 @@
         <v>36</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="84" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="B84" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>514</v>
-      </c>
       <c r="D84" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F84" s="3">
         <v>0.5</v>
@@ -4430,47 +4436,47 @@
         <v>36</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="B85" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>526</v>
-      </c>
       <c r="D85" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F85" s="1">
         <v>0.5</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>36</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="86" spans="1:9" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86" s="4" t="s">
         <v>530</v>
       </c>
-      <c r="B86" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C86" s="4" t="s">
+      <c r="D86" s="4" t="s">
         <v>531</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>532</v>
       </c>
       <c r="F86" s="3">
         <v>0.5</v>
@@ -4482,21 +4488,21 @@
         <v>36</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="87" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="B87" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C87" s="4" t="s">
+      <c r="D87" s="4" t="s">
         <v>539</v>
-      </c>
-      <c r="D87" s="4" t="s">
-        <v>540</v>
       </c>
       <c r="F87" s="3">
         <v>0.5</v>
@@ -4508,21 +4514,21 @@
         <v>36</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="88" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C88" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="B88" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C88" s="4" t="s">
+      <c r="D88" s="4" t="s">
         <v>542</v>
-      </c>
-      <c r="D88" s="4" t="s">
-        <v>543</v>
       </c>
       <c r="F88" s="3">
         <v>0.5</v>
@@ -4534,21 +4540,21 @@
         <v>36</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="89" spans="1:9" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C89" s="4" t="s">
         <v>544</v>
       </c>
-      <c r="B89" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C89" s="4" t="s">
+      <c r="D89" s="4" t="s">
         <v>545</v>
-      </c>
-      <c r="D89" s="4" t="s">
-        <v>546</v>
       </c>
       <c r="F89" s="3">
         <v>1</v>
@@ -4560,21 +4566,21 @@
         <v>36</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="90" spans="1:9" s="3" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="D90" s="4" t="s">
         <v>547</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>545</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>548</v>
       </c>
       <c r="F90" s="3">
         <v>1</v>
@@ -4586,53 +4592,76 @@
         <v>36</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A91" s="6" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>574</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>578</v>
+      </c>
+      <c r="F91" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I91" s="3" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" s="3" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="B91" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C91" s="7" t="s">
+      <c r="B92" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="D92" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="D91" s="7" t="s">
+      <c r="F92" s="3">
+        <v>1</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A93" s="6" t="s">
         <v>581</v>
       </c>
-      <c r="F91" s="6">
+      <c r="B93" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>583</v>
+      </c>
+      <c r="F93" s="6">
         <v>0.5</v>
       </c>
-      <c r="H91" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I91" s="6" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
-        <v>579</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>580</v>
-      </c>
-      <c r="D92" s="7" t="s">
-        <v>582</v>
-      </c>
-      <c r="F92" s="6">
-        <v>1</v>
-      </c>
-      <c r="H92" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I92" s="6" t="s">
-        <v>578</v>
+      <c r="H93" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I93" s="6" t="s">
+        <v>584</v>
       </c>
     </row>
   </sheetData>
@@ -4649,8 +4678,8 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A41" sqref="A41:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4905,7 +4934,7 @@
         <v>421</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -5590,7 +5619,7 @@
         <v>378</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F39" s="1">
         <v>1</v>
@@ -5633,7 +5662,7 @@
         <v>500</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>502</v>
+        <v>580</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -5641,7 +5670,7 @@
         <v>501</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>502</v>
+        <v>580</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -5790,16 +5819,16 @@
     </row>
     <row r="49" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C49" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>519</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>520</v>
       </c>
       <c r="F49" s="3">
         <v>2</v>
@@ -5808,27 +5837,27 @@
         <v>36</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B50" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C50" s="15" t="s">
+        <v>521</v>
+      </c>
+      <c r="D50" s="15" t="s">
         <v>522</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="F50" s="14">
+        <v>3</v>
+      </c>
+      <c r="G50" s="14" t="s">
         <v>523</v>
-      </c>
-      <c r="F50" s="14">
-        <v>3</v>
-      </c>
-      <c r="G50" s="14" t="s">
-        <v>524</v>
       </c>
       <c r="H50" s="14" t="s">
         <v>36</v>
@@ -5836,16 +5865,16 @@
     </row>
     <row r="51" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C51" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>534</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>535</v>
       </c>
       <c r="F51" s="3">
         <v>1</v>
@@ -5859,16 +5888,16 @@
     </row>
     <row r="52" spans="1:9" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C52" s="7" t="s">
+        <v>535</v>
+      </c>
+      <c r="D52" s="7" t="s">
         <v>536</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>537</v>
       </c>
       <c r="F52" s="6">
         <v>0.5</v>
@@ -5879,16 +5908,16 @@
     </row>
     <row r="53" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C53" s="4" t="s">
+        <v>550</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>551</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>552</v>
       </c>
       <c r="F53" s="3">
         <v>0.5</v>
@@ -6161,7 +6190,7 @@
         <v>38</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -6184,7 +6213,7 @@
         <v>36</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -6374,7 +6403,7 @@
         <v>325</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="F18" s="3">
         <v>1</v>
@@ -6463,7 +6492,7 @@
         <v>475</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F22" s="3">
         <v>1</v>
@@ -6593,13 +6622,13 @@
         <v>77</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F4" s="14">
         <v>50</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>36</v>
@@ -6619,7 +6648,7 @@
         <v>240</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F5" s="3">
         <v>2</v>
@@ -6642,7 +6671,7 @@
         <v>260</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F6" s="3">
         <v>2</v>
@@ -6671,7 +6700,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>36</v>
@@ -6720,7 +6749,7 @@
         <v>5</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>36</v>
@@ -6754,16 +6783,16 @@
     </row>
     <row r="11" spans="1:9" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>83</v>
       </c>
       <c r="C11" s="15" t="s">
+        <v>516</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>517</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>518</v>
       </c>
       <c r="F11" s="14">
         <f>20*12</f>
@@ -6773,7 +6802,7 @@
         <v>37</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified FractureDipSet.Mean_MF_HalfLength() to check for MFP30=0 and if so returning zero (B87). Not yet tested.
</commit_message>
<xml_diff>
--- a/Documentation/WorkToDo.xlsx
+++ b/Documentation/WorkToDo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MWelch\source\repos\DFMGenerator_Code\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joint\source\repos\DFMGenerator_Code\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF43E88F-0727-4CD2-9875-044A4E05515C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B99B5A-9B34-4D72-ACA8-C68326844282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bug fixes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="588">
   <si>
     <t>Type</t>
   </si>
@@ -1974,7 +1974,16 @@
     <t>When multistage Petrel models are run with fractures growing within each gridblock in between output stages, the output centrelines are consistently longer than the fracture patches in the early output stages. This problem does not affect output files, in which the centrelines are consistent with the fracture patches. This is because the copies of the global DFN that are made at the end of each stage contain links to the still active local MacrofractureSegmentIJK objects rather than inactive copies of these; if the segments subsequently grow, these longer versions will be used to populate the centrelines in the Petrel model (which is done after the explicit DFN growth has run to completion). The problem can be solved by creating a list of XYZ centrepoints within the MacrofractureXYZ object and populating this in the PopulateData function, as the fracture patch cornerpoints are; since this is called at the end of each stage, it will populate it with the centrepoint locations at that time.</t>
   </si>
   <si>
-    <t>For Release 2.2.3</t>
+    <t>B87</t>
+  </si>
+  <si>
+    <t>Not populating Mean Fracture Length property in implicit Petrel models where fracture density is zero</t>
+  </si>
+  <si>
+    <t>The Mean Fracture Length property in implicit Petrel fracture models should be populated with "zero" values in gridblocks where the fracture density is zero, but instead it is being populated with null values. This is because it tries to calculate the length by dividing MFP32/(MFP30*h), but this will return NaN if both MFP32 and MFP30 are zero. Can be solved by modifying  FractureDipSet.Mean_MF_HalfLength() to check for MFP30=0 and if so returning zero.</t>
+  </si>
+  <si>
+    <t>Done: Needs testing</t>
   </si>
 </sst>
 </file>
@@ -2403,11 +2412,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I93"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D92" sqref="D92"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I95" sqref="I95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4641,27 +4650,50 @@
         <v>562</v>
       </c>
     </row>
-    <row r="93" spans="1:9" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A93" s="6" t="s">
+    <row r="93" spans="1:9" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
         <v>581</v>
       </c>
-      <c r="B93" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C93" s="7" t="s">
+      <c r="B93" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C93" s="4" t="s">
         <v>582</v>
       </c>
-      <c r="D93" s="7" t="s">
+      <c r="D93" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="F93" s="6">
+      <c r="F93" s="3">
         <v>0.5</v>
       </c>
-      <c r="H93" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I93" s="6" t="s">
+      <c r="H93" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I93" s="3" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A94" s="6" t="s">
         <v>584</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>585</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>586</v>
+      </c>
+      <c r="F94" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H94" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I94" s="6" t="s">
+        <v>587</v>
       </c>
     </row>
   </sheetData>
@@ -4678,7 +4710,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A41" sqref="A41:XFD42"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modified FractureSet.Calculate_MeanPropagationDistance() so that when it checks the mean propagation rate is greater than zero, it converts to a float to eliminate rounding errors; this prevents it from returning infinite values (B88). Also modified FractureDipSet.calculateTotalMacrofracturePopulation() and FractureDipSet.calculateCumulativeMacrofracturePopulationArrays() to calculate zero values and increments for P30 and P32 fracture densities if the fracture sets are not activated, and modified FractureDipSet.setMacrofractureDeactivationRate() to more efficiently calculate the mean active fracture half length by not looking up the MFP30 density twice.
</commit_message>
<xml_diff>
--- a/Documentation/WorkToDo.xlsx
+++ b/Documentation/WorkToDo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joint\source\repos\DFMGenerator_Code\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B99B5A-9B34-4D72-ACA8-C68326844282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C29078-7B10-4092-95B3-020C1B46E5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="590">
   <si>
     <t>Type</t>
   </si>
@@ -1983,7 +1983,13 @@
     <t>The Mean Fracture Length property in implicit Petrel fracture models should be populated with "zero" values in gridblocks where the fracture density is zero, but instead it is being populated with null values. This is because it tries to calculate the length by dividing MFP32/(MFP30*h), but this will return NaN if both MFP32 and MFP30 are zero. Can be solved by modifying  FractureDipSet.Mean_MF_HalfLength() to check for MFP30=0 and if so returning zero.</t>
   </si>
   <si>
-    <t>Done: Needs testing</t>
+    <t>B88</t>
+  </si>
+  <si>
+    <t>Generating NaN values for MFP30 and MFP32 values in certain cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is still generating NaN values for a_MFP30 and a_MFP32 for residual active fracture sets in certain specific conditions. This occurs when the propagation rate is very low but not quite zero but FII is zero, FractureSet.Calculate_MeanPropagationDistance() returns an infinite value and FractureDipSet.calculateTotalMacrofracturePopulation throws a Nan when calculating tsK_a_MFP30_value for residual active fractures. Can be fixed by modifying FractureSet.Calculate_MeanPropagationDistance() so that when it checks the mean propagation rate is greater than zero, it converts to a float to eliminate rounding errors. </t>
   </si>
 </sst>
 </file>
@@ -2412,11 +2418,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:I95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I95" sqref="I95"/>
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4673,27 +4679,50 @@
         <v>562</v>
       </c>
     </row>
-    <row r="94" spans="1:9" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A94" s="6" t="s">
+    <row r="94" spans="1:9" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="B94" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C94" s="7" t="s">
+      <c r="B94" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C94" s="4" t="s">
         <v>585</v>
       </c>
-      <c r="D94" s="7" t="s">
+      <c r="D94" s="4" t="s">
         <v>586</v>
       </c>
-      <c r="F94" s="6">
+      <c r="F94" s="3">
         <v>0.1</v>
       </c>
-      <c r="H94" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I94" s="6" t="s">
+      <c r="H94" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I94" s="3" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
         <v>587</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>588</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="F95" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H95" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I95" s="3" t="s">
+        <v>562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a check for dChiMP_dChiTot_K > 0 when calculating  StressShadowDecreaseFactor in FractureDipSet.calculateTotalMacrofracturePopulation(), and otherwise returning zero (B89).
</commit_message>
<xml_diff>
--- a/Documentation/WorkToDo.xlsx
+++ b/Documentation/WorkToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joint\source\repos\DFMGenerator_Code\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C29078-7B10-4092-95B3-020C1B46E5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F645B64-5FCA-4441-90F8-06C6C2BB9028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="592">
   <si>
     <t>Type</t>
   </si>
@@ -1989,7 +1989,13 @@
     <t>Generating NaN values for MFP30 and MFP32 values in certain cells</t>
   </si>
   <si>
-    <t xml:space="preserve">It is still generating NaN values for a_MFP30 and a_MFP32 for residual active fracture sets in certain specific conditions. This occurs when the propagation rate is very low but not quite zero but FII is zero, FractureSet.Calculate_MeanPropagationDistance() returns an infinite value and FractureDipSet.calculateTotalMacrofracturePopulation throws a Nan when calculating tsK_a_MFP30_value for residual active fractures. Can be fixed by modifying FractureSet.Calculate_MeanPropagationDistance() so that when it checks the mean propagation rate is greater than zero, it converts to a float to eliminate rounding errors. </t>
+    <t xml:space="preserve">It is still generating NaN values for a_MFP30 and a_MFP32 for residual active fracture sets in certain specific conditions. This occurs when the propagation rate is very low but not quite zero but FII is zero, FractureSet.Calculate_MeanPropagationDistance() returns an infinite value and FractureDipSet.calculateTotalMacrofracturePopulation() throws a Nan when calculating tsK_a_MFP30_value for residual active fractures. Can be fixed by modifying FractureSet.Calculate_MeanPropagationDistance() so that when it checks the mean propagation rate is greater than zero, it converts to a float to eliminate rounding errors. </t>
+  </si>
+  <si>
+    <t>It is still generating NaN values for a_MFP30 and a_MFP32 for residual active fracture sets in certain specific conditions. This occurs in zero-length timesteps (which can happen in multistage models where the final deformation episode has indefinite length but no fractures are active), and FractureDipSet.calculateTotalMacrofracturePopulation() throws a Nan when calculating ts_StressShadowDecreaseFactor because bot the numerator and denominator of the exponent can be zero. This can be prevented by adding a check for dChiMP_dChiTot_K &gt; 0 when calculating  StressShadowDecreaseFactor, and otherwise returning zero.</t>
+  </si>
+  <si>
+    <t>B89</t>
   </si>
 </sst>
 </file>
@@ -2418,11 +2424,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D93" sqref="D93"/>
+      <selection pane="bottomLeft" activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4722,6 +4728,29 @@
         <v>36</v>
       </c>
       <c r="I95" s="3" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>588</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="F96" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I96" s="3" t="s">
         <v>562</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified PointXYZ.getCrossoverPoint()  to include a check for the minimum angle between the two lines; if it is less than the specified angular tolerance, the lines will be considered parallel and the function will return null (B84)
</commit_message>
<xml_diff>
--- a/Documentation/WorkToDo.xlsx
+++ b/Documentation/WorkToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joint\source\repos\DFMGenerator_Code\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F645B64-5FCA-4441-90F8-06C6C2BB9028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56D33A9-8DF0-4D1F-BC88-AB5BD6639530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1956,9 +1956,6 @@
     <t>When run with oblique fracture sets, it often generates small patches at the edges of gridblocks with very intense, closely spaced fracture segments. It appears that these are mostly relay segments rather than propagating segments; the intense zones contain only one or two fractures, but these are made up of very short segments connected by relay zones. The patches represent gaps between the stress shadows of primary fractures and the edges of the grid, or between the stress shadows of misaligned primary fractures in adjacent gridblocks, where only later non-optimally aligned fractures can grow. This cannot be prevented; however the relay zones often cross each other. This problem can be fixed by modifying FractureSet.checkStressShadowInteraction() to not create relay zones if a third fracture lies between the two fracture tips. It was also necessary to add relay fracture segments to the list of local macrofracture segments in eash fracture set object (although not the list of MacrofractureSegmentHolders in each gridblock object) to allow cross-checking.</t>
   </si>
   <si>
-    <t>When run with oblique fracture sets, it occasionally still produces "spiking" factures (where one or more cornerpoints lies way outside the model bounds). This is due to trying to bevel against a nearly parallel intersecting fracture segment edges. Rewritten MacrofractureXYZ.PopulateData() and PointXYZ.getCrossoverPoint() to allow limits to the bevelling relative to the fracture segment against which it is bevelled (both for intersecting fractures and other segments of the same fracture), rather than using a minimum angle cutoff.</t>
-  </si>
-  <si>
     <t>This is due to the new code that allows the fracture dipset evolution stage to revert from Residual to Growing in FractureDipSet.calculateTotalMacrofracturePopulation(). When this happened it was not resetting the density increments to zero. This was especially a problem for the s_MFP30_increment, which was getting multiplied by the timestep duration twice and leading to very large increments. This has been fixed, but still need to check if 1) does this also affect calculateMacrofractureArrays() fn?, 2) Does this problem occur anywhere else, 3) When and why does the state sometimes oscillate between Residual and Growing, even with no vertical extension?, 4) A few cells (e.g. 24,21 in Gullfaks Tarbert 2) still do not form secondary sets in the new code, whereas they did in the old.  This occurs because the test for switching from Growing to Residual (residual aMFP30 &gt; growing aMFP30) is not the same as the test for reverting from Residual to Growing (maximum propagation length in timestep &gt; mean propagation length before deactivating). Modified the code so it does not revert from ResidualActive to Growing within the calculateTotalMacrofracturePopulation() function, but instead within the fds.checkStressShadowWidthChange() function, only if the stress shadow width has changed.</t>
   </si>
   <si>
@@ -1996,6 +1993,9 @@
   </si>
   <si>
     <t>B89</t>
+  </si>
+  <si>
+    <t>When run with oblique fracture sets, it occasionally still produces "spiking" factures (where one or more cornerpoints lies way outside the model bounds). This is due to trying to bevel against a nearly parallel intersecting fracture segment edges. Rewritten MacrofractureXYZ.PopulateData() and PointXYZ.getCrossoverPoint() to allow limits to the bevelling relative to the fracture segment against which it is bevelled (both for intersecting fractures and other segments of the same fracture), and incorporate the minimum angle cutoff check into PointXYZ.getCrossoverPoint().</t>
   </si>
 </sst>
 </file>
@@ -2427,8 +2427,8 @@
   <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D95" sqref="D95"/>
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4393,7 +4393,7 @@
         <v>508</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F82" s="3">
         <v>1</v>
@@ -4627,7 +4627,7 @@
         <v>574</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>578</v>
+        <v>591</v>
       </c>
       <c r="F91" s="3">
         <v>0.5</v>
@@ -4664,16 +4664,16 @@
     </row>
     <row r="93" spans="1:9" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C93" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="B93" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C93" s="4" t="s">
+      <c r="D93" s="4" t="s">
         <v>582</v>
-      </c>
-      <c r="D93" s="4" t="s">
-        <v>583</v>
       </c>
       <c r="F93" s="3">
         <v>0.5</v>
@@ -4687,16 +4687,16 @@
     </row>
     <row r="94" spans="1:9" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C94" s="4" t="s">
         <v>584</v>
       </c>
-      <c r="B94" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C94" s="4" t="s">
+      <c r="D94" s="4" t="s">
         <v>585</v>
-      </c>
-      <c r="D94" s="4" t="s">
-        <v>586</v>
       </c>
       <c r="F94" s="3">
         <v>0.1</v>
@@ -4710,16 +4710,16 @@
     </row>
     <row r="95" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C95" s="4" t="s">
         <v>587</v>
       </c>
-      <c r="B95" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C95" s="4" t="s">
+      <c r="D95" s="4" t="s">
         <v>588</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>589</v>
       </c>
       <c r="F95" s="3">
         <v>0.5</v>
@@ -4733,16 +4733,16 @@
     </row>
     <row r="96" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F96" s="3">
         <v>0.2</v>
@@ -5752,7 +5752,7 @@
         <v>500</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -5760,7 +5760,7 @@
         <v>501</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modified the PropagationControl object to assign a default value for the azimuth of fracture set zero which will be used if the load tensors for all deformation episodes are isotropic, and modified main() (for the standalone version) and ExecuteSimple() (for the Petrel plugin) to set this to the specified minimum horizontal strain azimuth for the first deformation episode. This prevents the fracture orienation defaulting to E-W if another minimum horizontal strain orientation is specified but the strain load is isotropic (B90).
Also added DFM_Plotter_6set_Centrelines.xlsm to data analysis spreadsheet collection.
</commit_message>
<xml_diff>
--- a/Documentation/WorkToDo.xlsx
+++ b/Documentation/WorkToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joint\source\repos\DFMGenerator_Code\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56D33A9-8DF0-4D1F-BC88-AB5BD6639530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC132EC9-5B33-4634-B6FF-461D46EBCAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="595">
   <si>
     <t>Type</t>
   </si>
@@ -1996,6 +1996,15 @@
   </si>
   <si>
     <t>When run with oblique fracture sets, it occasionally still produces "spiking" factures (where one or more cornerpoints lies way outside the model bounds). This is due to trying to bevel against a nearly parallel intersecting fracture segment edges. Rewritten MacrofractureXYZ.PopulateData() and PointXYZ.getCrossoverPoint() to allow limits to the bevelling relative to the fracture segment against which it is bevelled (both for intersecting fractures and other segments of the same fracture), and incorporate the minimum angle cutoff check into PointXYZ.getCrossoverPoint().</t>
+  </si>
+  <si>
+    <t>B90</t>
+  </si>
+  <si>
+    <t>Setting fracture orientation to E-W if isotropic horizontal strain load is defined</t>
+  </si>
+  <si>
+    <t>If the horizontal strain load is isotropic, the azimuth of set 0 fractures will be set to zero degrees (i.e. E-W striking fractures) even if a different ehmin azimuth is specified. This is because it takes the orientation from minimum principal component of the strain (or stress) load tensor, which gives an azimuth of 0 by default if the tensor is isotropic. This can be solved by assigning a default value in the PropagationControl object which will be used if the load tensors for all deformation episodes are isotropic, and setting this to the specified minimum horizontal strain azimuth for the first deformation episode.</t>
   </si>
 </sst>
 </file>
@@ -2424,11 +2433,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I96"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D91" sqref="D91"/>
+      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4751,6 +4760,29 @@
         <v>36</v>
       </c>
       <c r="I96" s="3" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>593</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="F97" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I97" s="3" t="s">
         <v>562</v>
       </c>
     </row>

</xml_diff>